<commit_message>
expanded CScene class to parse more settings from ini file
</commit_message>
<xml_diff>
--- a/assets/mappings/TileMappings.xlsx
+++ b/assets/mappings/TileMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Project\MDS Stuff\July2021\2D Programming\2DGame-Assessment3\SimpleWars\assets\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E1F122-C2A8-4503-9C1B-E65FD7555E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E0AD7E-C227-4B90-B2BD-7887BFB1380A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26175" yWindow="5865" windowWidth="20835" windowHeight="18780" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
+    <workbookView xWindow="13320" yWindow="1200" windowWidth="20835" windowHeight="18780" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
   </bookViews>
   <sheets>
     <sheet name="MountainVillage" sheetId="1" r:id="rId1"/>
@@ -68,105 +68,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -575,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8450DF45-5C77-496B-BFAF-6D0E8F617C52}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="A18" sqref="A18:Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1946,32 +1848,139 @@
         <v>106</v>
       </c>
     </row>
+    <row r="18" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>106</v>
+      </c>
+      <c r="B18">
+        <v>106</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>11</v>
+      </c>
+      <c r="G18">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>11</v>
+      </c>
+      <c r="L18">
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <v>73</v>
+      </c>
+      <c r="N18">
+        <v>11</v>
+      </c>
+      <c r="O18">
+        <v>11</v>
+      </c>
+      <c r="P18">
+        <v>11</v>
+      </c>
+      <c r="Q18">
+        <v>11</v>
+      </c>
+      <c r="R18">
+        <v>11</v>
+      </c>
+      <c r="S18">
+        <v>11</v>
+      </c>
+      <c r="T18">
+        <v>11</v>
+      </c>
+      <c r="U18">
+        <v>11</v>
+      </c>
+      <c r="V18">
+        <v>11</v>
+      </c>
+      <c r="W18">
+        <v>11</v>
+      </c>
+      <c r="X18">
+        <v>11</v>
+      </c>
+      <c r="Y18">
+        <v>106</v>
+      </c>
+      <c r="Z18">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z17">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>106</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:Z18">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>11</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>80</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
-      <formula>50</formula>
-      <formula>55</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>60</formula>
-      <formula>65</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>70</formula>
-      <formula>73</formula>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
-Implemented main menu to select 1/2 playter mode -Implemented auto AI placement of units
</commit_message>
<xml_diff>
--- a/assets/mappings/TileMappings.xlsx
+++ b/assets/mappings/TileMappings.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Project\MDS Stuff\July2021\2D Programming\2DGame-Assessment3\SimpleWars\assets\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E0AD7E-C227-4B90-B2BD-7887BFB1380A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E54A8D1-35B0-442F-84E7-632638EEE6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="1200" windowWidth="20835" windowHeight="18780" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
+    <workbookView xWindow="15405" yWindow="1725" windowWidth="20835" windowHeight="18780" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
   </bookViews>
   <sheets>
-    <sheet name="MountainVillage" sheetId="1" r:id="rId1"/>
+    <sheet name="MainMenu" sheetId="2" r:id="rId1"/>
+    <sheet name="MountainVillage" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -68,7 +69,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -121,7 +171,28 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -142,28 +213,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -476,11 +526,1496 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1ED720-4874-4A90-B1AC-63934A65A0A1}">
+  <dimension ref="A1:Z18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:Z18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>74</v>
+      </c>
+      <c r="B1">
+        <v>74</v>
+      </c>
+      <c r="C1">
+        <v>74</v>
+      </c>
+      <c r="D1">
+        <v>74</v>
+      </c>
+      <c r="E1">
+        <v>74</v>
+      </c>
+      <c r="F1">
+        <v>74</v>
+      </c>
+      <c r="G1">
+        <v>74</v>
+      </c>
+      <c r="H1">
+        <v>74</v>
+      </c>
+      <c r="I1">
+        <v>74</v>
+      </c>
+      <c r="J1">
+        <v>74</v>
+      </c>
+      <c r="K1">
+        <v>74</v>
+      </c>
+      <c r="L1">
+        <v>74</v>
+      </c>
+      <c r="M1">
+        <v>74</v>
+      </c>
+      <c r="N1">
+        <v>74</v>
+      </c>
+      <c r="O1">
+        <v>74</v>
+      </c>
+      <c r="P1">
+        <v>74</v>
+      </c>
+      <c r="Q1">
+        <v>74</v>
+      </c>
+      <c r="R1">
+        <v>74</v>
+      </c>
+      <c r="S1">
+        <v>74</v>
+      </c>
+      <c r="T1">
+        <v>74</v>
+      </c>
+      <c r="U1">
+        <v>74</v>
+      </c>
+      <c r="V1">
+        <v>74</v>
+      </c>
+      <c r="W1">
+        <v>74</v>
+      </c>
+      <c r="X1">
+        <v>74</v>
+      </c>
+      <c r="Y1">
+        <v>74</v>
+      </c>
+      <c r="Z1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>74</v>
+      </c>
+      <c r="C2">
+        <v>74</v>
+      </c>
+      <c r="D2">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <v>74</v>
+      </c>
+      <c r="F2">
+        <v>74</v>
+      </c>
+      <c r="G2">
+        <v>74</v>
+      </c>
+      <c r="H2">
+        <v>74</v>
+      </c>
+      <c r="I2">
+        <v>74</v>
+      </c>
+      <c r="J2">
+        <v>74</v>
+      </c>
+      <c r="K2">
+        <v>74</v>
+      </c>
+      <c r="L2">
+        <v>74</v>
+      </c>
+      <c r="M2">
+        <v>74</v>
+      </c>
+      <c r="N2">
+        <v>74</v>
+      </c>
+      <c r="O2">
+        <v>74</v>
+      </c>
+      <c r="P2">
+        <v>74</v>
+      </c>
+      <c r="Q2">
+        <v>74</v>
+      </c>
+      <c r="R2">
+        <v>74</v>
+      </c>
+      <c r="S2">
+        <v>74</v>
+      </c>
+      <c r="T2">
+        <v>74</v>
+      </c>
+      <c r="U2">
+        <v>74</v>
+      </c>
+      <c r="V2">
+        <v>74</v>
+      </c>
+      <c r="W2">
+        <v>74</v>
+      </c>
+      <c r="X2">
+        <v>74</v>
+      </c>
+      <c r="Y2">
+        <v>74</v>
+      </c>
+      <c r="Z2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>74</v>
+      </c>
+      <c r="C3">
+        <v>74</v>
+      </c>
+      <c r="D3">
+        <v>74</v>
+      </c>
+      <c r="E3">
+        <v>74</v>
+      </c>
+      <c r="F3">
+        <v>74</v>
+      </c>
+      <c r="G3">
+        <v>74</v>
+      </c>
+      <c r="H3">
+        <v>74</v>
+      </c>
+      <c r="I3">
+        <v>74</v>
+      </c>
+      <c r="J3">
+        <v>74</v>
+      </c>
+      <c r="K3">
+        <v>74</v>
+      </c>
+      <c r="L3">
+        <v>74</v>
+      </c>
+      <c r="M3">
+        <v>74</v>
+      </c>
+      <c r="N3">
+        <v>74</v>
+      </c>
+      <c r="O3">
+        <v>74</v>
+      </c>
+      <c r="P3">
+        <v>74</v>
+      </c>
+      <c r="Q3">
+        <v>74</v>
+      </c>
+      <c r="R3">
+        <v>74</v>
+      </c>
+      <c r="S3">
+        <v>74</v>
+      </c>
+      <c r="T3">
+        <v>74</v>
+      </c>
+      <c r="U3">
+        <v>74</v>
+      </c>
+      <c r="V3">
+        <v>74</v>
+      </c>
+      <c r="W3">
+        <v>74</v>
+      </c>
+      <c r="X3">
+        <v>74</v>
+      </c>
+      <c r="Y3">
+        <v>74</v>
+      </c>
+      <c r="Z3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>74</v>
+      </c>
+      <c r="C4">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>74</v>
+      </c>
+      <c r="E4">
+        <v>74</v>
+      </c>
+      <c r="F4">
+        <v>74</v>
+      </c>
+      <c r="G4">
+        <v>74</v>
+      </c>
+      <c r="H4">
+        <v>74</v>
+      </c>
+      <c r="I4">
+        <v>74</v>
+      </c>
+      <c r="J4">
+        <v>74</v>
+      </c>
+      <c r="K4">
+        <v>74</v>
+      </c>
+      <c r="L4">
+        <v>74</v>
+      </c>
+      <c r="M4">
+        <v>74</v>
+      </c>
+      <c r="N4">
+        <v>74</v>
+      </c>
+      <c r="O4">
+        <v>74</v>
+      </c>
+      <c r="P4">
+        <v>74</v>
+      </c>
+      <c r="Q4">
+        <v>74</v>
+      </c>
+      <c r="R4">
+        <v>74</v>
+      </c>
+      <c r="S4">
+        <v>74</v>
+      </c>
+      <c r="T4">
+        <v>74</v>
+      </c>
+      <c r="U4">
+        <v>74</v>
+      </c>
+      <c r="V4">
+        <v>74</v>
+      </c>
+      <c r="W4">
+        <v>74</v>
+      </c>
+      <c r="X4">
+        <v>74</v>
+      </c>
+      <c r="Y4">
+        <v>74</v>
+      </c>
+      <c r="Z4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>74</v>
+      </c>
+      <c r="B5">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <v>74</v>
+      </c>
+      <c r="E5">
+        <v>74</v>
+      </c>
+      <c r="F5">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <v>74</v>
+      </c>
+      <c r="H5">
+        <v>74</v>
+      </c>
+      <c r="I5">
+        <v>74</v>
+      </c>
+      <c r="J5">
+        <v>74</v>
+      </c>
+      <c r="K5">
+        <v>74</v>
+      </c>
+      <c r="L5">
+        <v>74</v>
+      </c>
+      <c r="M5">
+        <v>74</v>
+      </c>
+      <c r="N5">
+        <v>74</v>
+      </c>
+      <c r="O5">
+        <v>74</v>
+      </c>
+      <c r="P5">
+        <v>74</v>
+      </c>
+      <c r="Q5">
+        <v>74</v>
+      </c>
+      <c r="R5">
+        <v>74</v>
+      </c>
+      <c r="S5">
+        <v>74</v>
+      </c>
+      <c r="T5">
+        <v>74</v>
+      </c>
+      <c r="U5">
+        <v>74</v>
+      </c>
+      <c r="V5">
+        <v>74</v>
+      </c>
+      <c r="W5">
+        <v>74</v>
+      </c>
+      <c r="X5">
+        <v>74</v>
+      </c>
+      <c r="Y5">
+        <v>74</v>
+      </c>
+      <c r="Z5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>74</v>
+      </c>
+      <c r="B6">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>74</v>
+      </c>
+      <c r="D6">
+        <v>74</v>
+      </c>
+      <c r="E6">
+        <v>74</v>
+      </c>
+      <c r="F6">
+        <v>74</v>
+      </c>
+      <c r="G6">
+        <v>74</v>
+      </c>
+      <c r="H6">
+        <v>74</v>
+      </c>
+      <c r="I6">
+        <v>74</v>
+      </c>
+      <c r="J6">
+        <v>74</v>
+      </c>
+      <c r="K6">
+        <v>74</v>
+      </c>
+      <c r="L6">
+        <v>74</v>
+      </c>
+      <c r="M6">
+        <v>74</v>
+      </c>
+      <c r="N6">
+        <v>74</v>
+      </c>
+      <c r="O6">
+        <v>74</v>
+      </c>
+      <c r="P6">
+        <v>74</v>
+      </c>
+      <c r="Q6">
+        <v>74</v>
+      </c>
+      <c r="R6">
+        <v>74</v>
+      </c>
+      <c r="S6">
+        <v>74</v>
+      </c>
+      <c r="T6">
+        <v>74</v>
+      </c>
+      <c r="U6">
+        <v>74</v>
+      </c>
+      <c r="V6">
+        <v>74</v>
+      </c>
+      <c r="W6">
+        <v>74</v>
+      </c>
+      <c r="X6">
+        <v>74</v>
+      </c>
+      <c r="Y6">
+        <v>74</v>
+      </c>
+      <c r="Z6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>74</v>
+      </c>
+      <c r="F7">
+        <v>74</v>
+      </c>
+      <c r="G7">
+        <v>74</v>
+      </c>
+      <c r="H7">
+        <v>74</v>
+      </c>
+      <c r="I7">
+        <v>74</v>
+      </c>
+      <c r="J7">
+        <v>74</v>
+      </c>
+      <c r="K7">
+        <v>74</v>
+      </c>
+      <c r="L7">
+        <v>74</v>
+      </c>
+      <c r="M7">
+        <v>74</v>
+      </c>
+      <c r="N7">
+        <v>74</v>
+      </c>
+      <c r="O7">
+        <v>74</v>
+      </c>
+      <c r="P7">
+        <v>74</v>
+      </c>
+      <c r="Q7">
+        <v>74</v>
+      </c>
+      <c r="R7">
+        <v>74</v>
+      </c>
+      <c r="S7">
+        <v>74</v>
+      </c>
+      <c r="T7">
+        <v>74</v>
+      </c>
+      <c r="U7">
+        <v>74</v>
+      </c>
+      <c r="V7">
+        <v>74</v>
+      </c>
+      <c r="W7">
+        <v>74</v>
+      </c>
+      <c r="X7">
+        <v>74</v>
+      </c>
+      <c r="Y7">
+        <v>74</v>
+      </c>
+      <c r="Z7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <v>74</v>
+      </c>
+      <c r="F8">
+        <v>74</v>
+      </c>
+      <c r="G8">
+        <v>74</v>
+      </c>
+      <c r="H8">
+        <v>74</v>
+      </c>
+      <c r="I8">
+        <v>74</v>
+      </c>
+      <c r="J8">
+        <v>74</v>
+      </c>
+      <c r="K8">
+        <v>74</v>
+      </c>
+      <c r="L8">
+        <v>74</v>
+      </c>
+      <c r="M8">
+        <v>74</v>
+      </c>
+      <c r="N8">
+        <v>74</v>
+      </c>
+      <c r="O8">
+        <v>74</v>
+      </c>
+      <c r="P8">
+        <v>74</v>
+      </c>
+      <c r="Q8">
+        <v>74</v>
+      </c>
+      <c r="R8">
+        <v>74</v>
+      </c>
+      <c r="S8">
+        <v>74</v>
+      </c>
+      <c r="T8">
+        <v>74</v>
+      </c>
+      <c r="U8">
+        <v>74</v>
+      </c>
+      <c r="V8">
+        <v>74</v>
+      </c>
+      <c r="W8">
+        <v>74</v>
+      </c>
+      <c r="X8">
+        <v>74</v>
+      </c>
+      <c r="Y8">
+        <v>74</v>
+      </c>
+      <c r="Z8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>74</v>
+      </c>
+      <c r="C9">
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>74</v>
+      </c>
+      <c r="E9">
+        <v>74</v>
+      </c>
+      <c r="F9">
+        <v>74</v>
+      </c>
+      <c r="G9">
+        <v>74</v>
+      </c>
+      <c r="H9">
+        <v>74</v>
+      </c>
+      <c r="I9">
+        <v>74</v>
+      </c>
+      <c r="J9">
+        <v>74</v>
+      </c>
+      <c r="K9">
+        <v>74</v>
+      </c>
+      <c r="L9">
+        <v>74</v>
+      </c>
+      <c r="M9">
+        <v>74</v>
+      </c>
+      <c r="N9">
+        <v>74</v>
+      </c>
+      <c r="O9">
+        <v>74</v>
+      </c>
+      <c r="P9">
+        <v>74</v>
+      </c>
+      <c r="Q9">
+        <v>74</v>
+      </c>
+      <c r="R9">
+        <v>74</v>
+      </c>
+      <c r="S9">
+        <v>74</v>
+      </c>
+      <c r="T9">
+        <v>74</v>
+      </c>
+      <c r="U9">
+        <v>74</v>
+      </c>
+      <c r="V9">
+        <v>74</v>
+      </c>
+      <c r="W9">
+        <v>74</v>
+      </c>
+      <c r="X9">
+        <v>74</v>
+      </c>
+      <c r="Y9">
+        <v>74</v>
+      </c>
+      <c r="Z9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>74</v>
+      </c>
+      <c r="B10">
+        <v>74</v>
+      </c>
+      <c r="C10">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>74</v>
+      </c>
+      <c r="E10">
+        <v>74</v>
+      </c>
+      <c r="F10">
+        <v>74</v>
+      </c>
+      <c r="G10">
+        <v>74</v>
+      </c>
+      <c r="H10">
+        <v>74</v>
+      </c>
+      <c r="I10">
+        <v>74</v>
+      </c>
+      <c r="J10">
+        <v>74</v>
+      </c>
+      <c r="K10">
+        <v>74</v>
+      </c>
+      <c r="L10">
+        <v>74</v>
+      </c>
+      <c r="M10">
+        <v>74</v>
+      </c>
+      <c r="N10">
+        <v>74</v>
+      </c>
+      <c r="O10">
+        <v>74</v>
+      </c>
+      <c r="P10">
+        <v>74</v>
+      </c>
+      <c r="Q10">
+        <v>74</v>
+      </c>
+      <c r="R10">
+        <v>74</v>
+      </c>
+      <c r="S10">
+        <v>74</v>
+      </c>
+      <c r="T10">
+        <v>74</v>
+      </c>
+      <c r="U10">
+        <v>74</v>
+      </c>
+      <c r="V10">
+        <v>74</v>
+      </c>
+      <c r="W10">
+        <v>74</v>
+      </c>
+      <c r="X10">
+        <v>74</v>
+      </c>
+      <c r="Y10">
+        <v>74</v>
+      </c>
+      <c r="Z10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>74</v>
+      </c>
+      <c r="B11">
+        <v>74</v>
+      </c>
+      <c r="C11">
+        <v>74</v>
+      </c>
+      <c r="D11">
+        <v>74</v>
+      </c>
+      <c r="E11">
+        <v>74</v>
+      </c>
+      <c r="F11">
+        <v>74</v>
+      </c>
+      <c r="G11">
+        <v>74</v>
+      </c>
+      <c r="H11">
+        <v>74</v>
+      </c>
+      <c r="I11">
+        <v>74</v>
+      </c>
+      <c r="J11">
+        <v>74</v>
+      </c>
+      <c r="K11">
+        <v>74</v>
+      </c>
+      <c r="L11">
+        <v>74</v>
+      </c>
+      <c r="M11">
+        <v>74</v>
+      </c>
+      <c r="N11">
+        <v>74</v>
+      </c>
+      <c r="O11">
+        <v>74</v>
+      </c>
+      <c r="P11">
+        <v>74</v>
+      </c>
+      <c r="Q11">
+        <v>74</v>
+      </c>
+      <c r="R11">
+        <v>74</v>
+      </c>
+      <c r="S11">
+        <v>74</v>
+      </c>
+      <c r="T11">
+        <v>74</v>
+      </c>
+      <c r="U11">
+        <v>74</v>
+      </c>
+      <c r="V11">
+        <v>74</v>
+      </c>
+      <c r="W11">
+        <v>74</v>
+      </c>
+      <c r="X11">
+        <v>74</v>
+      </c>
+      <c r="Y11">
+        <v>74</v>
+      </c>
+      <c r="Z11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>74</v>
+      </c>
+      <c r="B12">
+        <v>74</v>
+      </c>
+      <c r="C12">
+        <v>74</v>
+      </c>
+      <c r="D12">
+        <v>74</v>
+      </c>
+      <c r="E12">
+        <v>74</v>
+      </c>
+      <c r="F12">
+        <v>74</v>
+      </c>
+      <c r="G12">
+        <v>74</v>
+      </c>
+      <c r="H12">
+        <v>74</v>
+      </c>
+      <c r="I12">
+        <v>74</v>
+      </c>
+      <c r="J12">
+        <v>74</v>
+      </c>
+      <c r="K12">
+        <v>74</v>
+      </c>
+      <c r="L12">
+        <v>74</v>
+      </c>
+      <c r="M12">
+        <v>74</v>
+      </c>
+      <c r="N12">
+        <v>74</v>
+      </c>
+      <c r="O12">
+        <v>74</v>
+      </c>
+      <c r="P12">
+        <v>74</v>
+      </c>
+      <c r="Q12">
+        <v>74</v>
+      </c>
+      <c r="R12">
+        <v>74</v>
+      </c>
+      <c r="S12">
+        <v>74</v>
+      </c>
+      <c r="T12">
+        <v>74</v>
+      </c>
+      <c r="U12">
+        <v>74</v>
+      </c>
+      <c r="V12">
+        <v>74</v>
+      </c>
+      <c r="W12">
+        <v>74</v>
+      </c>
+      <c r="X12">
+        <v>74</v>
+      </c>
+      <c r="Y12">
+        <v>74</v>
+      </c>
+      <c r="Z12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <v>74</v>
+      </c>
+      <c r="D13">
+        <v>74</v>
+      </c>
+      <c r="E13">
+        <v>74</v>
+      </c>
+      <c r="F13">
+        <v>74</v>
+      </c>
+      <c r="G13">
+        <v>74</v>
+      </c>
+      <c r="H13">
+        <v>74</v>
+      </c>
+      <c r="I13">
+        <v>74</v>
+      </c>
+      <c r="J13">
+        <v>74</v>
+      </c>
+      <c r="K13">
+        <v>74</v>
+      </c>
+      <c r="L13">
+        <v>74</v>
+      </c>
+      <c r="M13">
+        <v>74</v>
+      </c>
+      <c r="N13">
+        <v>74</v>
+      </c>
+      <c r="O13">
+        <v>74</v>
+      </c>
+      <c r="P13">
+        <v>74</v>
+      </c>
+      <c r="Q13">
+        <v>74</v>
+      </c>
+      <c r="R13">
+        <v>74</v>
+      </c>
+      <c r="S13">
+        <v>74</v>
+      </c>
+      <c r="T13">
+        <v>74</v>
+      </c>
+      <c r="U13">
+        <v>74</v>
+      </c>
+      <c r="V13">
+        <v>74</v>
+      </c>
+      <c r="W13">
+        <v>74</v>
+      </c>
+      <c r="X13">
+        <v>74</v>
+      </c>
+      <c r="Y13">
+        <v>74</v>
+      </c>
+      <c r="Z13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>74</v>
+      </c>
+      <c r="B14">
+        <v>74</v>
+      </c>
+      <c r="C14">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>74</v>
+      </c>
+      <c r="E14">
+        <v>74</v>
+      </c>
+      <c r="F14">
+        <v>74</v>
+      </c>
+      <c r="G14">
+        <v>74</v>
+      </c>
+      <c r="H14">
+        <v>74</v>
+      </c>
+      <c r="I14">
+        <v>74</v>
+      </c>
+      <c r="J14">
+        <v>74</v>
+      </c>
+      <c r="K14">
+        <v>74</v>
+      </c>
+      <c r="L14">
+        <v>74</v>
+      </c>
+      <c r="M14">
+        <v>74</v>
+      </c>
+      <c r="N14">
+        <v>74</v>
+      </c>
+      <c r="O14">
+        <v>74</v>
+      </c>
+      <c r="P14">
+        <v>74</v>
+      </c>
+      <c r="Q14">
+        <v>74</v>
+      </c>
+      <c r="R14">
+        <v>74</v>
+      </c>
+      <c r="S14">
+        <v>74</v>
+      </c>
+      <c r="T14">
+        <v>74</v>
+      </c>
+      <c r="U14">
+        <v>74</v>
+      </c>
+      <c r="V14">
+        <v>74</v>
+      </c>
+      <c r="W14">
+        <v>74</v>
+      </c>
+      <c r="X14">
+        <v>74</v>
+      </c>
+      <c r="Y14">
+        <v>74</v>
+      </c>
+      <c r="Z14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>74</v>
+      </c>
+      <c r="B15">
+        <v>74</v>
+      </c>
+      <c r="C15">
+        <v>74</v>
+      </c>
+      <c r="D15">
+        <v>74</v>
+      </c>
+      <c r="E15">
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <v>74</v>
+      </c>
+      <c r="G15">
+        <v>74</v>
+      </c>
+      <c r="H15">
+        <v>74</v>
+      </c>
+      <c r="I15">
+        <v>74</v>
+      </c>
+      <c r="J15">
+        <v>74</v>
+      </c>
+      <c r="K15">
+        <v>74</v>
+      </c>
+      <c r="L15">
+        <v>74</v>
+      </c>
+      <c r="M15">
+        <v>74</v>
+      </c>
+      <c r="N15">
+        <v>74</v>
+      </c>
+      <c r="O15">
+        <v>74</v>
+      </c>
+      <c r="P15">
+        <v>74</v>
+      </c>
+      <c r="Q15">
+        <v>74</v>
+      </c>
+      <c r="R15">
+        <v>74</v>
+      </c>
+      <c r="S15">
+        <v>74</v>
+      </c>
+      <c r="T15">
+        <v>74</v>
+      </c>
+      <c r="U15">
+        <v>74</v>
+      </c>
+      <c r="V15">
+        <v>74</v>
+      </c>
+      <c r="W15">
+        <v>74</v>
+      </c>
+      <c r="X15">
+        <v>74</v>
+      </c>
+      <c r="Y15">
+        <v>74</v>
+      </c>
+      <c r="Z15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>74</v>
+      </c>
+      <c r="B16">
+        <v>74</v>
+      </c>
+      <c r="C16">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>74</v>
+      </c>
+      <c r="E16">
+        <v>74</v>
+      </c>
+      <c r="F16">
+        <v>74</v>
+      </c>
+      <c r="G16">
+        <v>74</v>
+      </c>
+      <c r="H16">
+        <v>74</v>
+      </c>
+      <c r="I16">
+        <v>74</v>
+      </c>
+      <c r="J16">
+        <v>74</v>
+      </c>
+      <c r="K16">
+        <v>74</v>
+      </c>
+      <c r="L16">
+        <v>74</v>
+      </c>
+      <c r="M16">
+        <v>74</v>
+      </c>
+      <c r="N16">
+        <v>74</v>
+      </c>
+      <c r="O16">
+        <v>74</v>
+      </c>
+      <c r="P16">
+        <v>74</v>
+      </c>
+      <c r="Q16">
+        <v>74</v>
+      </c>
+      <c r="R16">
+        <v>74</v>
+      </c>
+      <c r="S16">
+        <v>74</v>
+      </c>
+      <c r="T16">
+        <v>74</v>
+      </c>
+      <c r="U16">
+        <v>74</v>
+      </c>
+      <c r="V16">
+        <v>74</v>
+      </c>
+      <c r="W16">
+        <v>74</v>
+      </c>
+      <c r="X16">
+        <v>74</v>
+      </c>
+      <c r="Y16">
+        <v>74</v>
+      </c>
+      <c r="Z16">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <v>74</v>
+      </c>
+      <c r="E17">
+        <v>74</v>
+      </c>
+      <c r="F17">
+        <v>74</v>
+      </c>
+      <c r="G17">
+        <v>74</v>
+      </c>
+      <c r="H17">
+        <v>74</v>
+      </c>
+      <c r="I17">
+        <v>74</v>
+      </c>
+      <c r="J17">
+        <v>74</v>
+      </c>
+      <c r="K17">
+        <v>74</v>
+      </c>
+      <c r="L17">
+        <v>74</v>
+      </c>
+      <c r="M17">
+        <v>74</v>
+      </c>
+      <c r="N17">
+        <v>74</v>
+      </c>
+      <c r="O17">
+        <v>74</v>
+      </c>
+      <c r="P17">
+        <v>74</v>
+      </c>
+      <c r="Q17">
+        <v>74</v>
+      </c>
+      <c r="R17">
+        <v>74</v>
+      </c>
+      <c r="S17">
+        <v>74</v>
+      </c>
+      <c r="T17">
+        <v>74</v>
+      </c>
+      <c r="U17">
+        <v>74</v>
+      </c>
+      <c r="V17">
+        <v>74</v>
+      </c>
+      <c r="W17">
+        <v>74</v>
+      </c>
+      <c r="X17">
+        <v>74</v>
+      </c>
+      <c r="Y17">
+        <v>74</v>
+      </c>
+      <c r="Z17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>74</v>
+      </c>
+      <c r="B18">
+        <v>74</v>
+      </c>
+      <c r="C18">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>74</v>
+      </c>
+      <c r="E18">
+        <v>74</v>
+      </c>
+      <c r="F18">
+        <v>74</v>
+      </c>
+      <c r="G18">
+        <v>74</v>
+      </c>
+      <c r="H18">
+        <v>74</v>
+      </c>
+      <c r="I18">
+        <v>74</v>
+      </c>
+      <c r="J18">
+        <v>74</v>
+      </c>
+      <c r="K18">
+        <v>74</v>
+      </c>
+      <c r="L18">
+        <v>74</v>
+      </c>
+      <c r="M18">
+        <v>74</v>
+      </c>
+      <c r="N18">
+        <v>74</v>
+      </c>
+      <c r="O18">
+        <v>74</v>
+      </c>
+      <c r="P18">
+        <v>74</v>
+      </c>
+      <c r="Q18">
+        <v>74</v>
+      </c>
+      <c r="R18">
+        <v>74</v>
+      </c>
+      <c r="S18">
+        <v>74</v>
+      </c>
+      <c r="T18">
+        <v>74</v>
+      </c>
+      <c r="U18">
+        <v>74</v>
+      </c>
+      <c r="V18">
+        <v>74</v>
+      </c>
+      <c r="W18">
+        <v>74</v>
+      </c>
+      <c r="X18">
+        <v>74</v>
+      </c>
+      <c r="Y18">
+        <v>74</v>
+      </c>
+      <c r="Z18">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:Z18">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8450DF45-5C77-496B-BFAF-6D0E8F617C52}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:Z18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z18" sqref="A1:Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1957,29 +3492,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:Z18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
-Implemented mountain pass map
</commit_message>
<xml_diff>
--- a/assets/mappings/TileMappings.xlsx
+++ b/assets/mappings/TileMappings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Project\MDS Stuff\July2021\2D Programming\2DGame-Assessment3\SimpleWars\assets\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E54A8D1-35B0-442F-84E7-632638EEE6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1199CAB6-2D85-4DFF-A1B1-54DDAF2724E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15405" yWindow="1725" windowWidth="20835" windowHeight="18780" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
   </bookViews>
   <sheets>
     <sheet name="MainMenu" sheetId="2" r:id="rId1"/>
     <sheet name="MountainVillage" sheetId="1" r:id="rId2"/>
+    <sheet name="MountainPass" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -69,7 +70,399 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="77">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -529,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1ED720-4874-4A90-B1AC-63934A65A0A1}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A1:Z18"/>
     </sheetView>
   </sheetViews>
@@ -1980,29 +2373,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z18">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="8" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="9" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="10" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="11" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="12" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="13" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="14" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3465,60 +3858,1734 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z17">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="14" operator="equal">
       <formula>106</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="13" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="12" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="10" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="9" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="8" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:Z18">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="61" priority="2" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="60" priority="3" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="6" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="7" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0471A5B-141A-4393-8FF3-563345529594}">
+  <dimension ref="A1:Z18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>106</v>
+      </c>
+      <c r="B1">
+        <v>106</v>
+      </c>
+      <c r="C1">
+        <v>106</v>
+      </c>
+      <c r="D1">
+        <v>106</v>
+      </c>
+      <c r="E1">
+        <v>106</v>
+      </c>
+      <c r="F1">
+        <v>106</v>
+      </c>
+      <c r="G1">
+        <v>106</v>
+      </c>
+      <c r="H1">
+        <v>106</v>
+      </c>
+      <c r="I1">
+        <v>106</v>
+      </c>
+      <c r="J1">
+        <v>106</v>
+      </c>
+      <c r="K1">
+        <v>106</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>63</v>
+      </c>
+      <c r="N1">
+        <v>11</v>
+      </c>
+      <c r="O1">
+        <v>11</v>
+      </c>
+      <c r="P1">
+        <v>106</v>
+      </c>
+      <c r="Q1">
+        <v>106</v>
+      </c>
+      <c r="R1">
+        <v>106</v>
+      </c>
+      <c r="S1">
+        <v>106</v>
+      </c>
+      <c r="T1">
+        <v>106</v>
+      </c>
+      <c r="U1">
+        <v>106</v>
+      </c>
+      <c r="V1">
+        <v>106</v>
+      </c>
+      <c r="W1">
+        <v>106</v>
+      </c>
+      <c r="X1">
+        <v>106</v>
+      </c>
+      <c r="Y1">
+        <v>106</v>
+      </c>
+      <c r="Z1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>106</v>
+      </c>
+      <c r="C2">
+        <v>106</v>
+      </c>
+      <c r="D2">
+        <v>106</v>
+      </c>
+      <c r="E2">
+        <v>106</v>
+      </c>
+      <c r="F2">
+        <v>106</v>
+      </c>
+      <c r="G2">
+        <v>106</v>
+      </c>
+      <c r="H2">
+        <v>106</v>
+      </c>
+      <c r="I2">
+        <v>106</v>
+      </c>
+      <c r="J2">
+        <v>106</v>
+      </c>
+      <c r="K2">
+        <v>106</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>63</v>
+      </c>
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>106</v>
+      </c>
+      <c r="Q2">
+        <v>106</v>
+      </c>
+      <c r="R2">
+        <v>106</v>
+      </c>
+      <c r="S2">
+        <v>106</v>
+      </c>
+      <c r="T2">
+        <v>106</v>
+      </c>
+      <c r="U2">
+        <v>106</v>
+      </c>
+      <c r="V2">
+        <v>106</v>
+      </c>
+      <c r="W2">
+        <v>106</v>
+      </c>
+      <c r="X2">
+        <v>106</v>
+      </c>
+      <c r="Y2">
+        <v>106</v>
+      </c>
+      <c r="Z2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>106</v>
+      </c>
+      <c r="C3">
+        <v>106</v>
+      </c>
+      <c r="D3">
+        <v>106</v>
+      </c>
+      <c r="E3">
+        <v>106</v>
+      </c>
+      <c r="F3">
+        <v>106</v>
+      </c>
+      <c r="G3">
+        <v>106</v>
+      </c>
+      <c r="H3">
+        <v>106</v>
+      </c>
+      <c r="I3">
+        <v>106</v>
+      </c>
+      <c r="J3">
+        <v>106</v>
+      </c>
+      <c r="K3">
+        <v>106</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>63</v>
+      </c>
+      <c r="N3">
+        <v>11</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>106</v>
+      </c>
+      <c r="Q3">
+        <v>106</v>
+      </c>
+      <c r="R3">
+        <v>106</v>
+      </c>
+      <c r="S3">
+        <v>106</v>
+      </c>
+      <c r="T3">
+        <v>106</v>
+      </c>
+      <c r="U3">
+        <v>106</v>
+      </c>
+      <c r="V3">
+        <v>106</v>
+      </c>
+      <c r="W3">
+        <v>106</v>
+      </c>
+      <c r="X3">
+        <v>106</v>
+      </c>
+      <c r="Y3">
+        <v>106</v>
+      </c>
+      <c r="Z3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>106</v>
+      </c>
+      <c r="B4">
+        <v>106</v>
+      </c>
+      <c r="C4">
+        <v>106</v>
+      </c>
+      <c r="D4">
+        <v>106</v>
+      </c>
+      <c r="E4">
+        <v>106</v>
+      </c>
+      <c r="F4">
+        <v>106</v>
+      </c>
+      <c r="G4">
+        <v>106</v>
+      </c>
+      <c r="H4">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>106</v>
+      </c>
+      <c r="J4">
+        <v>106</v>
+      </c>
+      <c r="K4">
+        <v>106</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4">
+        <v>63</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <v>11</v>
+      </c>
+      <c r="P4">
+        <v>106</v>
+      </c>
+      <c r="Q4">
+        <v>106</v>
+      </c>
+      <c r="R4">
+        <v>106</v>
+      </c>
+      <c r="S4">
+        <v>106</v>
+      </c>
+      <c r="T4">
+        <v>106</v>
+      </c>
+      <c r="U4">
+        <v>106</v>
+      </c>
+      <c r="V4">
+        <v>106</v>
+      </c>
+      <c r="W4">
+        <v>106</v>
+      </c>
+      <c r="X4">
+        <v>106</v>
+      </c>
+      <c r="Y4">
+        <v>106</v>
+      </c>
+      <c r="Z4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>106</v>
+      </c>
+      <c r="C5">
+        <v>106</v>
+      </c>
+      <c r="D5">
+        <v>106</v>
+      </c>
+      <c r="E5">
+        <v>106</v>
+      </c>
+      <c r="F5">
+        <v>106</v>
+      </c>
+      <c r="G5">
+        <v>106</v>
+      </c>
+      <c r="H5">
+        <v>106</v>
+      </c>
+      <c r="I5">
+        <v>106</v>
+      </c>
+      <c r="J5">
+        <v>106</v>
+      </c>
+      <c r="K5">
+        <v>106</v>
+      </c>
+      <c r="L5">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>63</v>
+      </c>
+      <c r="N5">
+        <v>11</v>
+      </c>
+      <c r="O5">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>106</v>
+      </c>
+      <c r="Q5">
+        <v>106</v>
+      </c>
+      <c r="R5">
+        <v>106</v>
+      </c>
+      <c r="S5">
+        <v>106</v>
+      </c>
+      <c r="T5">
+        <v>106</v>
+      </c>
+      <c r="U5">
+        <v>106</v>
+      </c>
+      <c r="V5">
+        <v>106</v>
+      </c>
+      <c r="W5">
+        <v>106</v>
+      </c>
+      <c r="X5">
+        <v>106</v>
+      </c>
+      <c r="Y5">
+        <v>106</v>
+      </c>
+      <c r="Z5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>106</v>
+      </c>
+      <c r="C6">
+        <v>106</v>
+      </c>
+      <c r="D6">
+        <v>106</v>
+      </c>
+      <c r="E6">
+        <v>106</v>
+      </c>
+      <c r="F6">
+        <v>106</v>
+      </c>
+      <c r="G6">
+        <v>106</v>
+      </c>
+      <c r="H6">
+        <v>106</v>
+      </c>
+      <c r="I6">
+        <v>106</v>
+      </c>
+      <c r="J6">
+        <v>106</v>
+      </c>
+      <c r="K6">
+        <v>106</v>
+      </c>
+      <c r="L6">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>63</v>
+      </c>
+      <c r="N6">
+        <v>11</v>
+      </c>
+      <c r="O6">
+        <v>11</v>
+      </c>
+      <c r="P6">
+        <v>106</v>
+      </c>
+      <c r="Q6">
+        <v>106</v>
+      </c>
+      <c r="R6">
+        <v>106</v>
+      </c>
+      <c r="S6">
+        <v>106</v>
+      </c>
+      <c r="T6">
+        <v>106</v>
+      </c>
+      <c r="U6">
+        <v>106</v>
+      </c>
+      <c r="V6">
+        <v>106</v>
+      </c>
+      <c r="W6">
+        <v>106</v>
+      </c>
+      <c r="X6">
+        <v>106</v>
+      </c>
+      <c r="Y6">
+        <v>106</v>
+      </c>
+      <c r="Z6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>106</v>
+      </c>
+      <c r="D7">
+        <v>106</v>
+      </c>
+      <c r="E7">
+        <v>106</v>
+      </c>
+      <c r="F7">
+        <v>106</v>
+      </c>
+      <c r="G7">
+        <v>106</v>
+      </c>
+      <c r="H7">
+        <v>106</v>
+      </c>
+      <c r="I7">
+        <v>106</v>
+      </c>
+      <c r="J7">
+        <v>106</v>
+      </c>
+      <c r="K7">
+        <v>106</v>
+      </c>
+      <c r="L7">
+        <v>11</v>
+      </c>
+      <c r="M7">
+        <v>63</v>
+      </c>
+      <c r="N7">
+        <v>11</v>
+      </c>
+      <c r="O7">
+        <v>11</v>
+      </c>
+      <c r="P7">
+        <v>106</v>
+      </c>
+      <c r="Q7">
+        <v>106</v>
+      </c>
+      <c r="R7">
+        <v>106</v>
+      </c>
+      <c r="S7">
+        <v>106</v>
+      </c>
+      <c r="T7">
+        <v>106</v>
+      </c>
+      <c r="U7">
+        <v>106</v>
+      </c>
+      <c r="V7">
+        <v>106</v>
+      </c>
+      <c r="W7">
+        <v>106</v>
+      </c>
+      <c r="X7">
+        <v>106</v>
+      </c>
+      <c r="Y7">
+        <v>106</v>
+      </c>
+      <c r="Z7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8">
+        <v>106</v>
+      </c>
+      <c r="C8">
+        <v>106</v>
+      </c>
+      <c r="D8">
+        <v>106</v>
+      </c>
+      <c r="E8">
+        <v>106</v>
+      </c>
+      <c r="F8">
+        <v>106</v>
+      </c>
+      <c r="G8">
+        <v>106</v>
+      </c>
+      <c r="H8">
+        <v>106</v>
+      </c>
+      <c r="I8">
+        <v>106</v>
+      </c>
+      <c r="J8">
+        <v>106</v>
+      </c>
+      <c r="K8">
+        <v>106</v>
+      </c>
+      <c r="L8">
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <v>63</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
+      <c r="O8">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>106</v>
+      </c>
+      <c r="Q8">
+        <v>106</v>
+      </c>
+      <c r="R8">
+        <v>106</v>
+      </c>
+      <c r="S8">
+        <v>106</v>
+      </c>
+      <c r="T8">
+        <v>106</v>
+      </c>
+      <c r="U8">
+        <v>106</v>
+      </c>
+      <c r="V8">
+        <v>106</v>
+      </c>
+      <c r="W8">
+        <v>106</v>
+      </c>
+      <c r="X8">
+        <v>106</v>
+      </c>
+      <c r="Y8">
+        <v>106</v>
+      </c>
+      <c r="Z8">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>106</v>
+      </c>
+      <c r="B9">
+        <v>106</v>
+      </c>
+      <c r="C9">
+        <v>106</v>
+      </c>
+      <c r="D9">
+        <v>106</v>
+      </c>
+      <c r="E9">
+        <v>106</v>
+      </c>
+      <c r="F9">
+        <v>106</v>
+      </c>
+      <c r="G9">
+        <v>106</v>
+      </c>
+      <c r="H9">
+        <v>106</v>
+      </c>
+      <c r="I9">
+        <v>106</v>
+      </c>
+      <c r="J9">
+        <v>106</v>
+      </c>
+      <c r="K9">
+        <v>106</v>
+      </c>
+      <c r="L9">
+        <v>11</v>
+      </c>
+      <c r="M9">
+        <v>63</v>
+      </c>
+      <c r="N9">
+        <v>11</v>
+      </c>
+      <c r="O9">
+        <v>11</v>
+      </c>
+      <c r="P9">
+        <v>106</v>
+      </c>
+      <c r="Q9">
+        <v>106</v>
+      </c>
+      <c r="R9">
+        <v>106</v>
+      </c>
+      <c r="S9">
+        <v>106</v>
+      </c>
+      <c r="T9">
+        <v>106</v>
+      </c>
+      <c r="U9">
+        <v>106</v>
+      </c>
+      <c r="V9">
+        <v>106</v>
+      </c>
+      <c r="W9">
+        <v>106</v>
+      </c>
+      <c r="X9">
+        <v>106</v>
+      </c>
+      <c r="Y9">
+        <v>106</v>
+      </c>
+      <c r="Z9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>106</v>
+      </c>
+      <c r="B10">
+        <v>106</v>
+      </c>
+      <c r="C10">
+        <v>106</v>
+      </c>
+      <c r="D10">
+        <v>106</v>
+      </c>
+      <c r="E10">
+        <v>106</v>
+      </c>
+      <c r="F10">
+        <v>106</v>
+      </c>
+      <c r="G10">
+        <v>106</v>
+      </c>
+      <c r="H10">
+        <v>106</v>
+      </c>
+      <c r="I10">
+        <v>106</v>
+      </c>
+      <c r="J10">
+        <v>106</v>
+      </c>
+      <c r="K10">
+        <v>106</v>
+      </c>
+      <c r="L10">
+        <v>11</v>
+      </c>
+      <c r="M10">
+        <v>63</v>
+      </c>
+      <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>11</v>
+      </c>
+      <c r="P10">
+        <v>106</v>
+      </c>
+      <c r="Q10">
+        <v>106</v>
+      </c>
+      <c r="R10">
+        <v>106</v>
+      </c>
+      <c r="S10">
+        <v>106</v>
+      </c>
+      <c r="T10">
+        <v>106</v>
+      </c>
+      <c r="U10">
+        <v>106</v>
+      </c>
+      <c r="V10">
+        <v>106</v>
+      </c>
+      <c r="W10">
+        <v>106</v>
+      </c>
+      <c r="X10">
+        <v>106</v>
+      </c>
+      <c r="Y10">
+        <v>106</v>
+      </c>
+      <c r="Z10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>106</v>
+      </c>
+      <c r="C11">
+        <v>106</v>
+      </c>
+      <c r="D11">
+        <v>106</v>
+      </c>
+      <c r="E11">
+        <v>106</v>
+      </c>
+      <c r="F11">
+        <v>106</v>
+      </c>
+      <c r="G11">
+        <v>106</v>
+      </c>
+      <c r="H11">
+        <v>106</v>
+      </c>
+      <c r="I11">
+        <v>106</v>
+      </c>
+      <c r="J11">
+        <v>106</v>
+      </c>
+      <c r="K11">
+        <v>106</v>
+      </c>
+      <c r="L11">
+        <v>11</v>
+      </c>
+      <c r="M11">
+        <v>63</v>
+      </c>
+      <c r="N11">
+        <v>102</v>
+      </c>
+      <c r="O11">
+        <v>104</v>
+      </c>
+      <c r="P11">
+        <v>106</v>
+      </c>
+      <c r="Q11">
+        <v>106</v>
+      </c>
+      <c r="R11">
+        <v>106</v>
+      </c>
+      <c r="S11">
+        <v>106</v>
+      </c>
+      <c r="T11">
+        <v>106</v>
+      </c>
+      <c r="U11">
+        <v>106</v>
+      </c>
+      <c r="V11">
+        <v>106</v>
+      </c>
+      <c r="W11">
+        <v>106</v>
+      </c>
+      <c r="X11">
+        <v>106</v>
+      </c>
+      <c r="Y11">
+        <v>106</v>
+      </c>
+      <c r="Z11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>106</v>
+      </c>
+      <c r="B12">
+        <v>106</v>
+      </c>
+      <c r="C12">
+        <v>106</v>
+      </c>
+      <c r="D12">
+        <v>106</v>
+      </c>
+      <c r="E12">
+        <v>106</v>
+      </c>
+      <c r="F12">
+        <v>106</v>
+      </c>
+      <c r="G12">
+        <v>106</v>
+      </c>
+      <c r="H12">
+        <v>106</v>
+      </c>
+      <c r="I12">
+        <v>106</v>
+      </c>
+      <c r="J12">
+        <v>106</v>
+      </c>
+      <c r="K12">
+        <v>95</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12">
+        <v>101</v>
+      </c>
+      <c r="N12">
+        <v>94</v>
+      </c>
+      <c r="O12">
+        <v>105</v>
+      </c>
+      <c r="P12">
+        <v>106</v>
+      </c>
+      <c r="Q12">
+        <v>106</v>
+      </c>
+      <c r="R12">
+        <v>106</v>
+      </c>
+      <c r="S12">
+        <v>106</v>
+      </c>
+      <c r="T12">
+        <v>106</v>
+      </c>
+      <c r="U12">
+        <v>106</v>
+      </c>
+      <c r="V12">
+        <v>106</v>
+      </c>
+      <c r="W12">
+        <v>106</v>
+      </c>
+      <c r="X12">
+        <v>106</v>
+      </c>
+      <c r="Y12">
+        <v>106</v>
+      </c>
+      <c r="Z12">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>106</v>
+      </c>
+      <c r="B13">
+        <v>106</v>
+      </c>
+      <c r="C13">
+        <v>106</v>
+      </c>
+      <c r="D13">
+        <v>106</v>
+      </c>
+      <c r="E13">
+        <v>106</v>
+      </c>
+      <c r="F13">
+        <v>106</v>
+      </c>
+      <c r="G13">
+        <v>106</v>
+      </c>
+      <c r="H13">
+        <v>106</v>
+      </c>
+      <c r="I13">
+        <v>106</v>
+      </c>
+      <c r="J13">
+        <v>106</v>
+      </c>
+      <c r="K13">
+        <v>97</v>
+      </c>
+      <c r="L13">
+        <v>94</v>
+      </c>
+      <c r="M13">
+        <v>95</v>
+      </c>
+      <c r="N13">
+        <v>96</v>
+      </c>
+      <c r="O13">
+        <v>100</v>
+      </c>
+      <c r="P13">
+        <v>106</v>
+      </c>
+      <c r="Q13">
+        <v>106</v>
+      </c>
+      <c r="R13">
+        <v>106</v>
+      </c>
+      <c r="S13">
+        <v>106</v>
+      </c>
+      <c r="T13">
+        <v>106</v>
+      </c>
+      <c r="U13">
+        <v>106</v>
+      </c>
+      <c r="V13">
+        <v>106</v>
+      </c>
+      <c r="W13">
+        <v>106</v>
+      </c>
+      <c r="X13">
+        <v>106</v>
+      </c>
+      <c r="Y13">
+        <v>106</v>
+      </c>
+      <c r="Z13">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>106</v>
+      </c>
+      <c r="B14">
+        <v>106</v>
+      </c>
+      <c r="C14">
+        <v>106</v>
+      </c>
+      <c r="D14">
+        <v>106</v>
+      </c>
+      <c r="E14">
+        <v>106</v>
+      </c>
+      <c r="F14">
+        <v>106</v>
+      </c>
+      <c r="G14">
+        <v>106</v>
+      </c>
+      <c r="H14">
+        <v>106</v>
+      </c>
+      <c r="I14">
+        <v>106</v>
+      </c>
+      <c r="J14">
+        <v>106</v>
+      </c>
+      <c r="K14">
+        <v>102</v>
+      </c>
+      <c r="L14">
+        <v>104</v>
+      </c>
+      <c r="M14">
+        <v>63</v>
+      </c>
+      <c r="N14">
+        <v>120</v>
+      </c>
+      <c r="O14">
+        <v>121</v>
+      </c>
+      <c r="P14">
+        <v>121</v>
+      </c>
+      <c r="Q14">
+        <v>122</v>
+      </c>
+      <c r="R14">
+        <v>11</v>
+      </c>
+      <c r="S14">
+        <v>11</v>
+      </c>
+      <c r="T14">
+        <v>11</v>
+      </c>
+      <c r="U14">
+        <v>11</v>
+      </c>
+      <c r="V14">
+        <v>11</v>
+      </c>
+      <c r="W14">
+        <v>11</v>
+      </c>
+      <c r="X14">
+        <v>11</v>
+      </c>
+      <c r="Y14">
+        <v>11</v>
+      </c>
+      <c r="Z14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>106</v>
+      </c>
+      <c r="C15">
+        <v>106</v>
+      </c>
+      <c r="D15">
+        <v>106</v>
+      </c>
+      <c r="E15">
+        <v>106</v>
+      </c>
+      <c r="F15">
+        <v>106</v>
+      </c>
+      <c r="G15">
+        <v>106</v>
+      </c>
+      <c r="H15">
+        <v>106</v>
+      </c>
+      <c r="I15">
+        <v>106</v>
+      </c>
+      <c r="J15">
+        <v>106</v>
+      </c>
+      <c r="K15">
+        <v>102</v>
+      </c>
+      <c r="L15">
+        <v>104</v>
+      </c>
+      <c r="M15">
+        <v>63</v>
+      </c>
+      <c r="N15">
+        <v>120</v>
+      </c>
+      <c r="O15">
+        <v>121</v>
+      </c>
+      <c r="P15">
+        <v>121</v>
+      </c>
+      <c r="Q15">
+        <v>122</v>
+      </c>
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>11</v>
+      </c>
+      <c r="T15">
+        <v>11</v>
+      </c>
+      <c r="U15">
+        <v>11</v>
+      </c>
+      <c r="V15">
+        <v>11</v>
+      </c>
+      <c r="W15">
+        <v>11</v>
+      </c>
+      <c r="X15">
+        <v>11</v>
+      </c>
+      <c r="Y15">
+        <v>11</v>
+      </c>
+      <c r="Z15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>106</v>
+      </c>
+      <c r="B16">
+        <v>106</v>
+      </c>
+      <c r="C16">
+        <v>106</v>
+      </c>
+      <c r="D16">
+        <v>106</v>
+      </c>
+      <c r="E16">
+        <v>106</v>
+      </c>
+      <c r="F16">
+        <v>106</v>
+      </c>
+      <c r="G16">
+        <v>106</v>
+      </c>
+      <c r="H16">
+        <v>106</v>
+      </c>
+      <c r="I16">
+        <v>106</v>
+      </c>
+      <c r="J16">
+        <v>106</v>
+      </c>
+      <c r="K16">
+        <v>11</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>61</v>
+      </c>
+      <c r="N16">
+        <v>51</v>
+      </c>
+      <c r="O16">
+        <v>51</v>
+      </c>
+      <c r="P16">
+        <v>51</v>
+      </c>
+      <c r="Q16">
+        <v>51</v>
+      </c>
+      <c r="R16">
+        <v>51</v>
+      </c>
+      <c r="S16">
+        <v>51</v>
+      </c>
+      <c r="T16">
+        <v>51</v>
+      </c>
+      <c r="U16">
+        <v>51</v>
+      </c>
+      <c r="V16">
+        <v>51</v>
+      </c>
+      <c r="W16">
+        <v>51</v>
+      </c>
+      <c r="X16">
+        <v>51</v>
+      </c>
+      <c r="Y16">
+        <v>51</v>
+      </c>
+      <c r="Z16">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>106</v>
+      </c>
+      <c r="B17">
+        <v>106</v>
+      </c>
+      <c r="C17">
+        <v>106</v>
+      </c>
+      <c r="D17">
+        <v>106</v>
+      </c>
+      <c r="E17">
+        <v>106</v>
+      </c>
+      <c r="F17">
+        <v>106</v>
+      </c>
+      <c r="G17">
+        <v>106</v>
+      </c>
+      <c r="H17">
+        <v>106</v>
+      </c>
+      <c r="I17">
+        <v>106</v>
+      </c>
+      <c r="J17">
+        <v>106</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
+      </c>
+      <c r="L17">
+        <v>11</v>
+      </c>
+      <c r="M17">
+        <v>63</v>
+      </c>
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <v>21</v>
+      </c>
+      <c r="P17">
+        <v>21</v>
+      </c>
+      <c r="Q17">
+        <v>21</v>
+      </c>
+      <c r="R17">
+        <v>21</v>
+      </c>
+      <c r="S17">
+        <v>21</v>
+      </c>
+      <c r="T17">
+        <v>21</v>
+      </c>
+      <c r="U17">
+        <v>21</v>
+      </c>
+      <c r="V17">
+        <v>21</v>
+      </c>
+      <c r="W17">
+        <v>21</v>
+      </c>
+      <c r="X17">
+        <v>21</v>
+      </c>
+      <c r="Y17">
+        <v>21</v>
+      </c>
+      <c r="Z17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>106</v>
+      </c>
+      <c r="B18">
+        <v>106</v>
+      </c>
+      <c r="C18">
+        <v>106</v>
+      </c>
+      <c r="D18">
+        <v>106</v>
+      </c>
+      <c r="E18">
+        <v>106</v>
+      </c>
+      <c r="F18">
+        <v>106</v>
+      </c>
+      <c r="G18">
+        <v>106</v>
+      </c>
+      <c r="H18">
+        <v>106</v>
+      </c>
+      <c r="I18">
+        <v>106</v>
+      </c>
+      <c r="J18">
+        <v>106</v>
+      </c>
+      <c r="K18">
+        <v>11</v>
+      </c>
+      <c r="L18">
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <v>63</v>
+      </c>
+      <c r="N18">
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <v>80</v>
+      </c>
+      <c r="P18">
+        <v>80</v>
+      </c>
+      <c r="Q18">
+        <v>80</v>
+      </c>
+      <c r="R18">
+        <v>80</v>
+      </c>
+      <c r="S18">
+        <v>80</v>
+      </c>
+      <c r="T18">
+        <v>81</v>
+      </c>
+      <c r="U18">
+        <v>80</v>
+      </c>
+      <c r="V18">
+        <v>80</v>
+      </c>
+      <c r="W18">
+        <v>80</v>
+      </c>
+      <c r="X18">
+        <v>80</v>
+      </c>
+      <c r="Y18">
+        <v>80</v>
+      </c>
+      <c r="Z18">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A3:B17 A2:H2 L2:L5 P1:Q15 N2:Q5 M2:M18 A1:Q1 I8:K8 I10:K11">
+    <cfRule type="cellIs" dxfId="55" priority="50" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="51" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="55" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B18">
+    <cfRule type="cellIs" dxfId="48" priority="43" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="44" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="45" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="48" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="49" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:H18">
+    <cfRule type="cellIs" dxfId="41" priority="36" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:Z13">
+    <cfRule type="cellIs" dxfId="34" priority="29" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="34" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:S13">
+    <cfRule type="cellIs" dxfId="27" priority="22" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="27" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="28" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:K7 I12:J18 I9:K9">
+    <cfRule type="cellIs" dxfId="20" priority="15" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14:Z15">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:O15 K12:L18 N16:Z18 L6:L11">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Implemented bridge map --*found bug with move selector texture getting deleted
</commit_message>
<xml_diff>
--- a/assets/mappings/TileMappings.xlsx
+++ b/assets/mappings/TileMappings.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Project\MDS Stuff\July2021\2D Programming\2DGame-Assessment3\SimpleWars\assets\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1199CAB6-2D85-4DFF-A1B1-54DDAF2724E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2299353D-47F2-4D75-AE28-2BC176090EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{909D872D-8D2F-46DD-A7C8-B44B854B3BCA}"/>
   </bookViews>
   <sheets>
     <sheet name="MainMenu" sheetId="2" r:id="rId1"/>
     <sheet name="MountainVillage" sheetId="1" r:id="rId2"/>
     <sheet name="MountainPass" sheetId="3" r:id="rId3"/>
+    <sheet name="Bridge" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -70,7 +71,105 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="91">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2373,29 +2472,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z18">
-    <cfRule type="cellIs" dxfId="76" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="8" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="89" priority="9" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="88" priority="10" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="11" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="12" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="13" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="14" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2408,7 +2507,7 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z18" sqref="A1:Z18"/>
+      <selection sqref="A1:Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3858,56 +3957,56 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z17">
-    <cfRule type="cellIs" dxfId="69" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="14" operator="equal">
       <formula>106</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="82" priority="13" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="12" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="11" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="10" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="9" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="8" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:Z18">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="1" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="2" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="3" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="4" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="5" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="6" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="7" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3920,7 +4019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0471A5B-141A-4393-8FF3-563345529594}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -5371,168 +5470,1680 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B17 A2:H2 L2:L5 P1:Q15 N2:Q5 M2:M18 A1:Q1 I8:K8 I10:K11">
-    <cfRule type="cellIs" dxfId="55" priority="50" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="50" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="51" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="51" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="52" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="52" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="53" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="54" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="55" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="55" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="56" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:B18">
-    <cfRule type="cellIs" dxfId="48" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="43" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="44" operator="between">
+    <cfRule type="cellIs" dxfId="61" priority="44" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="between">
+    <cfRule type="cellIs" dxfId="60" priority="45" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="46" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="47" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="48" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="49" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:H18">
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="55" priority="36" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="54" priority="37" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="between">
+    <cfRule type="cellIs" dxfId="53" priority="38" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="39" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="40" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="between">
+    <cfRule type="cellIs" dxfId="50" priority="41" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="42" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:Z13">
-    <cfRule type="cellIs" dxfId="34" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="48" priority="29" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="47" priority="30" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="31" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="32" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="33" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S13">
-    <cfRule type="cellIs" dxfId="27" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="22" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="23" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="24" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="25" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="27" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K7 I12:J18 I9:K9">
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="15" operator="between">
       <formula>70</formula>
       <formula>73</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="between">
       <formula>60</formula>
       <formula>65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="between">
       <formula>50</formula>
       <formula>55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="18" operator="equal">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="between">
       <formula>102</formula>
       <formula>105</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:Z15">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:O15 K12:L18 N16:Z18 L6:L11">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="between">
+      <formula>70</formula>
+      <formula>73</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+      <formula>60</formula>
+      <formula>65</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="between">
+      <formula>50</formula>
+      <formula>55</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="between">
+      <formula>102</formula>
+      <formula>105</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>106</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC37CE7-7D0F-45B2-A639-6E0A3EFC0D4D}">
+  <dimension ref="A1:Z18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>106</v>
+      </c>
+      <c r="B1">
+        <v>106</v>
+      </c>
+      <c r="C1">
+        <v>12</v>
+      </c>
+      <c r="D1">
+        <v>80</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>63</v>
+      </c>
+      <c r="G1">
+        <v>11</v>
+      </c>
+      <c r="H1">
+        <v>11</v>
+      </c>
+      <c r="I1">
+        <v>11</v>
+      </c>
+      <c r="J1">
+        <v>11</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>11</v>
+      </c>
+      <c r="O1">
+        <v>11</v>
+      </c>
+      <c r="P1">
+        <v>11</v>
+      </c>
+      <c r="Q1">
+        <v>11</v>
+      </c>
+      <c r="R1">
+        <v>11</v>
+      </c>
+      <c r="S1">
+        <v>11</v>
+      </c>
+      <c r="T1">
+        <v>11</v>
+      </c>
+      <c r="U1">
+        <v>11</v>
+      </c>
+      <c r="V1">
+        <v>11</v>
+      </c>
+      <c r="W1">
+        <v>11</v>
+      </c>
+      <c r="X1">
+        <v>63</v>
+      </c>
+      <c r="Y1">
+        <v>11</v>
+      </c>
+      <c r="Z1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>106</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>63</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
+      <c r="I2">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>11</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>11</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2">
+        <v>11</v>
+      </c>
+      <c r="T2">
+        <v>11</v>
+      </c>
+      <c r="U2">
+        <v>11</v>
+      </c>
+      <c r="V2">
+        <v>11</v>
+      </c>
+      <c r="W2">
+        <v>11</v>
+      </c>
+      <c r="X2">
+        <v>63</v>
+      </c>
+      <c r="Y2">
+        <v>11</v>
+      </c>
+      <c r="Z2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>106</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>63</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>11</v>
+      </c>
+      <c r="N3">
+        <v>11</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>11</v>
+      </c>
+      <c r="Q3">
+        <v>11</v>
+      </c>
+      <c r="R3">
+        <v>11</v>
+      </c>
+      <c r="S3">
+        <v>11</v>
+      </c>
+      <c r="T3">
+        <v>11</v>
+      </c>
+      <c r="U3">
+        <v>11</v>
+      </c>
+      <c r="V3">
+        <v>11</v>
+      </c>
+      <c r="W3">
+        <v>11</v>
+      </c>
+      <c r="X3">
+        <v>63</v>
+      </c>
+      <c r="Y3">
+        <v>11</v>
+      </c>
+      <c r="Z3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>106</v>
+      </c>
+      <c r="B4">
+        <v>106</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>63</v>
+      </c>
+      <c r="G4">
+        <v>102</v>
+      </c>
+      <c r="H4">
+        <v>103</v>
+      </c>
+      <c r="I4">
+        <v>103</v>
+      </c>
+      <c r="J4">
+        <v>103</v>
+      </c>
+      <c r="K4">
+        <v>103</v>
+      </c>
+      <c r="L4">
+        <v>104</v>
+      </c>
+      <c r="M4">
+        <v>11</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <v>11</v>
+      </c>
+      <c r="P4">
+        <v>11</v>
+      </c>
+      <c r="Q4">
+        <v>11</v>
+      </c>
+      <c r="R4">
+        <v>11</v>
+      </c>
+      <c r="S4">
+        <v>11</v>
+      </c>
+      <c r="T4">
+        <v>11</v>
+      </c>
+      <c r="U4">
+        <v>11</v>
+      </c>
+      <c r="V4">
+        <v>11</v>
+      </c>
+      <c r="W4">
+        <v>11</v>
+      </c>
+      <c r="X4">
+        <v>63</v>
+      </c>
+      <c r="Y4">
+        <v>11</v>
+      </c>
+      <c r="Z4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>106</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>63</v>
+      </c>
+      <c r="G5">
+        <v>102</v>
+      </c>
+      <c r="H5">
+        <v>103</v>
+      </c>
+      <c r="I5">
+        <v>103</v>
+      </c>
+      <c r="J5">
+        <v>103</v>
+      </c>
+      <c r="K5">
+        <v>103</v>
+      </c>
+      <c r="L5">
+        <v>104</v>
+      </c>
+      <c r="M5">
+        <v>11</v>
+      </c>
+      <c r="N5">
+        <v>11</v>
+      </c>
+      <c r="O5">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>11</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
+      </c>
+      <c r="S5">
+        <v>11</v>
+      </c>
+      <c r="T5">
+        <v>11</v>
+      </c>
+      <c r="U5">
+        <v>11</v>
+      </c>
+      <c r="V5">
+        <v>11</v>
+      </c>
+      <c r="W5">
+        <v>11</v>
+      </c>
+      <c r="X5">
+        <v>63</v>
+      </c>
+      <c r="Y5">
+        <v>11</v>
+      </c>
+      <c r="Z5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>106</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>73</v>
+      </c>
+      <c r="G6">
+        <v>102</v>
+      </c>
+      <c r="H6">
+        <v>103</v>
+      </c>
+      <c r="I6">
+        <v>103</v>
+      </c>
+      <c r="J6">
+        <v>103</v>
+      </c>
+      <c r="K6">
+        <v>103</v>
+      </c>
+      <c r="L6">
+        <v>104</v>
+      </c>
+      <c r="M6">
+        <v>11</v>
+      </c>
+      <c r="N6">
+        <v>11</v>
+      </c>
+      <c r="O6">
+        <v>11</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>11</v>
+      </c>
+      <c r="R6">
+        <v>11</v>
+      </c>
+      <c r="S6">
+        <v>11</v>
+      </c>
+      <c r="T6">
+        <v>11</v>
+      </c>
+      <c r="U6">
+        <v>11</v>
+      </c>
+      <c r="V6">
+        <v>11</v>
+      </c>
+      <c r="W6">
+        <v>11</v>
+      </c>
+      <c r="X6">
+        <v>63</v>
+      </c>
+      <c r="Y6">
+        <v>11</v>
+      </c>
+      <c r="Z6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>21</v>
+      </c>
+      <c r="J7">
+        <v>21</v>
+      </c>
+      <c r="K7">
+        <v>21</v>
+      </c>
+      <c r="L7">
+        <v>21</v>
+      </c>
+      <c r="M7">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>130</v>
+      </c>
+      <c r="O7">
+        <v>131</v>
+      </c>
+      <c r="P7">
+        <v>131</v>
+      </c>
+      <c r="Q7">
+        <v>131</v>
+      </c>
+      <c r="R7">
+        <v>132</v>
+      </c>
+      <c r="S7">
+        <v>11</v>
+      </c>
+      <c r="T7">
+        <v>11</v>
+      </c>
+      <c r="U7">
+        <v>11</v>
+      </c>
+      <c r="V7">
+        <v>11</v>
+      </c>
+      <c r="W7">
+        <v>11</v>
+      </c>
+      <c r="X7">
+        <v>63</v>
+      </c>
+      <c r="Y7">
+        <v>11</v>
+      </c>
+      <c r="Z7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8">
+        <v>106</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>80</v>
+      </c>
+      <c r="H8">
+        <v>80</v>
+      </c>
+      <c r="I8">
+        <v>80</v>
+      </c>
+      <c r="J8">
+        <v>80</v>
+      </c>
+      <c r="K8">
+        <v>80</v>
+      </c>
+      <c r="L8">
+        <v>80</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>130</v>
+      </c>
+      <c r="O8">
+        <v>131</v>
+      </c>
+      <c r="P8">
+        <v>131</v>
+      </c>
+      <c r="Q8">
+        <v>131</v>
+      </c>
+      <c r="R8">
+        <v>132</v>
+      </c>
+      <c r="S8">
+        <v>11</v>
+      </c>
+      <c r="T8">
+        <v>11</v>
+      </c>
+      <c r="U8">
+        <v>11</v>
+      </c>
+      <c r="V8">
+        <v>11</v>
+      </c>
+      <c r="W8">
+        <v>11</v>
+      </c>
+      <c r="X8">
+        <v>63</v>
+      </c>
+      <c r="Y8">
+        <v>11</v>
+      </c>
+      <c r="Z8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>80</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>130</v>
+      </c>
+      <c r="O9">
+        <v>131</v>
+      </c>
+      <c r="P9">
+        <v>131</v>
+      </c>
+      <c r="Q9">
+        <v>131</v>
+      </c>
+      <c r="R9">
+        <v>132</v>
+      </c>
+      <c r="S9">
+        <v>11</v>
+      </c>
+      <c r="T9">
+        <v>11</v>
+      </c>
+      <c r="U9">
+        <v>11</v>
+      </c>
+      <c r="V9">
+        <v>11</v>
+      </c>
+      <c r="W9">
+        <v>11</v>
+      </c>
+      <c r="X9">
+        <v>63</v>
+      </c>
+      <c r="Y9">
+        <v>11</v>
+      </c>
+      <c r="Z9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>53</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>94</v>
+      </c>
+      <c r="I10">
+        <v>97</v>
+      </c>
+      <c r="J10">
+        <v>101</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>80</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>130</v>
+      </c>
+      <c r="O10">
+        <v>131</v>
+      </c>
+      <c r="P10">
+        <v>131</v>
+      </c>
+      <c r="Q10">
+        <v>131</v>
+      </c>
+      <c r="R10">
+        <v>132</v>
+      </c>
+      <c r="S10">
+        <v>11</v>
+      </c>
+      <c r="T10">
+        <v>11</v>
+      </c>
+      <c r="U10">
+        <v>11</v>
+      </c>
+      <c r="V10">
+        <v>11</v>
+      </c>
+      <c r="W10">
+        <v>11</v>
+      </c>
+      <c r="X10">
+        <v>63</v>
+      </c>
+      <c r="Y10">
+        <v>11</v>
+      </c>
+      <c r="Z10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>51</v>
+      </c>
+      <c r="E11">
+        <v>51</v>
+      </c>
+      <c r="F11">
+        <v>70</v>
+      </c>
+      <c r="G11">
+        <v>51</v>
+      </c>
+      <c r="H11">
+        <v>51</v>
+      </c>
+      <c r="I11">
+        <v>51</v>
+      </c>
+      <c r="J11">
+        <v>51</v>
+      </c>
+      <c r="K11">
+        <v>43</v>
+      </c>
+      <c r="L11">
+        <v>31</v>
+      </c>
+      <c r="M11">
+        <v>44</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>51</v>
+      </c>
+      <c r="P11">
+        <v>51</v>
+      </c>
+      <c r="Q11">
+        <v>51</v>
+      </c>
+      <c r="R11">
+        <v>51</v>
+      </c>
+      <c r="S11">
+        <v>62</v>
+      </c>
+      <c r="T11">
+        <v>51</v>
+      </c>
+      <c r="U11">
+        <v>51</v>
+      </c>
+      <c r="V11">
+        <v>51</v>
+      </c>
+      <c r="W11">
+        <v>51</v>
+      </c>
+      <c r="X11">
+        <v>71</v>
+      </c>
+      <c r="Y11">
+        <v>51</v>
+      </c>
+      <c r="Z11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>63</v>
+      </c>
+      <c r="G12">
+        <v>130</v>
+      </c>
+      <c r="H12">
+        <v>131</v>
+      </c>
+      <c r="I12">
+        <v>131</v>
+      </c>
+      <c r="J12">
+        <v>132</v>
+      </c>
+      <c r="K12">
+        <v>12</v>
+      </c>
+      <c r="L12">
+        <v>80</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>95</v>
+      </c>
+      <c r="P12">
+        <v>97</v>
+      </c>
+      <c r="Q12">
+        <v>96</v>
+      </c>
+      <c r="R12">
+        <v>101</v>
+      </c>
+      <c r="S12">
+        <v>63</v>
+      </c>
+      <c r="T12">
+        <v>102</v>
+      </c>
+      <c r="U12">
+        <v>103</v>
+      </c>
+      <c r="V12">
+        <v>104</v>
+      </c>
+      <c r="W12">
+        <v>106</v>
+      </c>
+      <c r="X12">
+        <v>106</v>
+      </c>
+      <c r="Y12">
+        <v>11</v>
+      </c>
+      <c r="Z12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>130</v>
+      </c>
+      <c r="H13">
+        <v>131</v>
+      </c>
+      <c r="I13">
+        <v>131</v>
+      </c>
+      <c r="J13">
+        <v>132</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>80</v>
+      </c>
+      <c r="M13">
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>21</v>
+      </c>
+      <c r="O13">
+        <v>21</v>
+      </c>
+      <c r="P13">
+        <v>21</v>
+      </c>
+      <c r="Q13">
+        <v>21</v>
+      </c>
+      <c r="R13">
+        <v>21</v>
+      </c>
+      <c r="S13">
+        <v>18</v>
+      </c>
+      <c r="T13">
+        <v>21</v>
+      </c>
+      <c r="U13">
+        <v>21</v>
+      </c>
+      <c r="V13">
+        <v>16</v>
+      </c>
+      <c r="W13">
+        <v>106</v>
+      </c>
+      <c r="X13">
+        <v>106</v>
+      </c>
+      <c r="Y13">
+        <v>11</v>
+      </c>
+      <c r="Z13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>130</v>
+      </c>
+      <c r="H14">
+        <v>131</v>
+      </c>
+      <c r="I14">
+        <v>131</v>
+      </c>
+      <c r="J14">
+        <v>132</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>80</v>
+      </c>
+      <c r="M14">
+        <v>80</v>
+      </c>
+      <c r="N14">
+        <v>80</v>
+      </c>
+      <c r="O14">
+        <v>80</v>
+      </c>
+      <c r="P14">
+        <v>80</v>
+      </c>
+      <c r="Q14">
+        <v>80</v>
+      </c>
+      <c r="R14">
+        <v>80</v>
+      </c>
+      <c r="S14">
+        <v>13</v>
+      </c>
+      <c r="T14">
+        <v>80</v>
+      </c>
+      <c r="U14">
+        <v>80</v>
+      </c>
+      <c r="V14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>106</v>
+      </c>
+      <c r="X14">
+        <v>106</v>
+      </c>
+      <c r="Y14">
+        <v>11</v>
+      </c>
+      <c r="Z14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>63</v>
+      </c>
+      <c r="G15">
+        <v>130</v>
+      </c>
+      <c r="H15">
+        <v>131</v>
+      </c>
+      <c r="I15">
+        <v>131</v>
+      </c>
+      <c r="J15">
+        <v>132</v>
+      </c>
+      <c r="K15">
+        <v>25</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>28</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>80</v>
+      </c>
+      <c r="V15">
+        <v>10</v>
+      </c>
+      <c r="W15">
+        <v>106</v>
+      </c>
+      <c r="X15">
+        <v>106</v>
+      </c>
+      <c r="Y15">
+        <v>11</v>
+      </c>
+      <c r="Z15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>63</v>
+      </c>
+      <c r="G16">
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>11</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>11</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>11</v>
+      </c>
+      <c r="N16">
+        <v>102</v>
+      </c>
+      <c r="O16">
+        <v>103</v>
+      </c>
+      <c r="P16">
+        <v>103</v>
+      </c>
+      <c r="Q16">
+        <v>103</v>
+      </c>
+      <c r="R16">
+        <v>104</v>
+      </c>
+      <c r="S16">
+        <v>63</v>
+      </c>
+      <c r="T16">
+        <v>12</v>
+      </c>
+      <c r="U16">
+        <v>80</v>
+      </c>
+      <c r="V16">
+        <v>10</v>
+      </c>
+      <c r="W16">
+        <v>106</v>
+      </c>
+      <c r="X16">
+        <v>106</v>
+      </c>
+      <c r="Y16">
+        <v>11</v>
+      </c>
+      <c r="Z16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>63</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>11</v>
+      </c>
+      <c r="I17">
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <v>11</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
+      </c>
+      <c r="L17">
+        <v>11</v>
+      </c>
+      <c r="M17">
+        <v>11</v>
+      </c>
+      <c r="N17">
+        <v>102</v>
+      </c>
+      <c r="O17">
+        <v>103</v>
+      </c>
+      <c r="P17">
+        <v>103</v>
+      </c>
+      <c r="Q17">
+        <v>103</v>
+      </c>
+      <c r="R17">
+        <v>104</v>
+      </c>
+      <c r="S17">
+        <v>63</v>
+      </c>
+      <c r="T17">
+        <v>12</v>
+      </c>
+      <c r="U17">
+        <v>80</v>
+      </c>
+      <c r="V17">
+        <v>10</v>
+      </c>
+      <c r="W17">
+        <v>106</v>
+      </c>
+      <c r="X17">
+        <v>106</v>
+      </c>
+      <c r="Y17">
+        <v>11</v>
+      </c>
+      <c r="Z17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>63</v>
+      </c>
+      <c r="G18">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>11</v>
+      </c>
+      <c r="L18">
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <v>11</v>
+      </c>
+      <c r="N18">
+        <v>102</v>
+      </c>
+      <c r="O18">
+        <v>103</v>
+      </c>
+      <c r="P18">
+        <v>103</v>
+      </c>
+      <c r="Q18">
+        <v>103</v>
+      </c>
+      <c r="R18">
+        <v>104</v>
+      </c>
+      <c r="S18">
+        <v>63</v>
+      </c>
+      <c r="T18">
+        <v>12</v>
+      </c>
+      <c r="U18">
+        <v>80</v>
+      </c>
+      <c r="V18">
+        <v>10</v>
+      </c>
+      <c r="W18">
+        <v>106</v>
+      </c>
+      <c r="X18">
+        <v>106</v>
+      </c>
+      <c r="Y18">
+        <v>11</v>
+      </c>
+      <c r="Z18">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:Z18">
     <cfRule type="cellIs" dxfId="13" priority="8" operator="between">
       <formula>70</formula>
       <formula>73</formula>
@@ -5559,7 +7170,7 @@
       <formula>106</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6:O15 K12:L18 N16:Z18 L6:L11">
+  <conditionalFormatting sqref="V12:W17 A18:Z18 X12:X18 V17:V18">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
       <formula>70</formula>
       <formula>73</formula>

</xml_diff>